<commit_message>
ccdc dataset icdc changes
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_Datasets.xlsx
+++ b/InputFiles/CCDC_Datasets.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4FB454-3D80-4597-A0AD-87297CE3EF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A931369-AA5B-45CE-A203-75030579C75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetPage" sheetId="1" r:id="rId1"/>
+    <sheet name="CoreAdditional" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>suffixUrl</t>
   </si>
@@ -58,13 +59,72 @@
   </si>
   <si>
     <t>DatasetScope</t>
+  </si>
+  <si>
+    <t>261200800001E-12-0-40
+Therapeutically Applicable Research to Generate Effective Treatments (TARGET) 
+HHSN261200800001E
+NCI Contract 
+U10CA180886
+COG NCTN Network Group Operations Center</t>
+  </si>
+  <si>
+    <t>phs000464</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino (212); Not Hispanic or Latino (546); Unknown (33)</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native (3); Asian (39); Black or African American (58); Native Hawaiian or Other Pacific Islander (2); White (579); Unknown (110)</t>
+  </si>
+  <si>
+    <t>0 to 4 years (248); 5 to 9 years (126); 10 to 14 years (252); 15 to 19 years (152); 20 to 24 years (11); 25 to 29 years (2)</t>
+  </si>
+  <si>
+    <t>Female (361); Male (430)</t>
+  </si>
+  <si>
+    <t>Intramural Research Program of the Center for Cancer Research, NCI</t>
+  </si>
+  <si>
+    <t>phs001928</t>
+  </si>
+  <si>
+    <t>Not Reported (267)</t>
+  </si>
+  <si>
+    <t>Pediatric and Young Adult (&lt;40 years) (267)</t>
+  </si>
+  <si>
+    <t>grant</t>
+  </si>
+  <si>
+    <t>dbgapID</t>
+  </si>
+  <si>
+    <t>noOfSamples</t>
+  </si>
+  <si>
+    <t>caseEthn</t>
+  </si>
+  <si>
+    <t>caseRace</t>
+  </si>
+  <si>
+    <t>caseAge</t>
+  </si>
+  <si>
+    <t>caseSex</t>
+  </si>
+  <si>
+    <t>numOfCases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +139,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212529"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +168,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -388,19 +460,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -428,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -448,4 +520,128 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F901FF4-9BBA-4DA7-BB49-1970CDDA0297}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.1796875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>267</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2">
+        <v>401</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>791</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://datacatalog-qa.ccdi.cancer.gov/dataset/dbGaP-phs001928" xr:uid="{5AB6D7DE-4005-48D0-BF08-408F543F0CCF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CCDC dataset script and icdc programs scripts
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_Datasets.xlsx
+++ b/InputFiles/CCDC_Datasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\March\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A931369-AA5B-45CE-A203-75030579C75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B5A48-8ED4-4D17-93E0-AAF5BEC571DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>suffixUrl</t>
   </si>
@@ -61,70 +61,76 @@
     <t>DatasetScope</t>
   </si>
   <si>
+    <t>phs000464</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino (212); Not Hispanic or Latino (546); Unknown (33)</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native (3); Asian (39); Black or African American (58); Native Hawaiian or Other Pacific Islander (2); White (579); Unknown (110)</t>
+  </si>
+  <si>
+    <t>0 to 4 years (248); 5 to 9 years (126); 10 to 14 years (252); 15 to 19 years (152); 20 to 24 years (11); 25 to 29 years (2)</t>
+  </si>
+  <si>
+    <t>Female (361); Male (430)</t>
+  </si>
+  <si>
+    <t>Intramural Research Program of the Center for Cancer Research, NCI</t>
+  </si>
+  <si>
+    <t>phs001928</t>
+  </si>
+  <si>
+    <t>Not Reported (267)</t>
+  </si>
+  <si>
+    <t>grant</t>
+  </si>
+  <si>
+    <t>dbgapID</t>
+  </si>
+  <si>
+    <t>noOfSamples</t>
+  </si>
+  <si>
+    <t>caseEthn</t>
+  </si>
+  <si>
+    <t>caseRace</t>
+  </si>
+  <si>
+    <t>caseAge</t>
+  </si>
+  <si>
+    <t>caseSex</t>
+  </si>
+  <si>
+    <t>numOfCases</t>
+  </si>
+  <si>
     <t>261200800001E-12-0-40
-Therapeutically Applicable Research to Generate Effective Treatments (TARGET) 
+Therapeutically Applicable Research to Generate Effective Treatments (TARGET)
 HHSN261200800001E
-NCI Contract 
+NCI Contract
 U10CA180886
 COG NCTN Network Group Operations Center</t>
   </si>
   <si>
-    <t>phs000464</t>
-  </si>
-  <si>
-    <t>Hispanic or Latino (212); Not Hispanic or Latino (546); Unknown (33)</t>
-  </si>
-  <si>
-    <t>American Indian or Alaska Native (3); Asian (39); Black or African American (58); Native Hawaiian or Other Pacific Islander (2); White (579); Unknown (110)</t>
-  </si>
-  <si>
-    <t>0 to 4 years (248); 5 to 9 years (126); 10 to 14 years (252); 15 to 19 years (152); 20 to 24 years (11); 25 to 29 years (2)</t>
-  </si>
-  <si>
-    <t>Female (361); Male (430)</t>
-  </si>
-  <si>
-    <t>Intramural Research Program of the Center for Cancer Research, NCI</t>
-  </si>
-  <si>
-    <t>phs001928</t>
-  </si>
-  <si>
-    <t>Not Reported (267)</t>
-  </si>
-  <si>
-    <t>Pediatric and Young Adult (&lt;40 years) (267)</t>
-  </si>
-  <si>
-    <t>grant</t>
-  </si>
-  <si>
-    <t>dbgapID</t>
-  </si>
-  <si>
-    <t>noOfSamples</t>
-  </si>
-  <si>
-    <t>caseEthn</t>
-  </si>
-  <si>
-    <t>caseRace</t>
-  </si>
-  <si>
-    <t>caseAge</t>
-  </si>
-  <si>
-    <t>caseSex</t>
-  </si>
-  <si>
-    <t>numOfCases</t>
+    <t>Pediatric and Young Adult (&lt;40 years) (267)</t>
+  </si>
+  <si>
+    <t>ResourceCode</t>
+  </si>
+  <si>
+    <t>grantInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,12 +145,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212529"/>
-      <name val="Lato"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,7 +176,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,15 +463,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -524,27 +523,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F901FF4-9BBA-4DA7-BB49-1970CDDA0297}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.1796875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="52.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" style="2" customWidth="1"/>
+    <col min="7" max="8" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,76 +553,85 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
         <v>267</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2">
         <v>401</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
         <v>791</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -630,11 +640,14 @@
       <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>